<commit_message>
Updating with public release
</commit_message>
<xml_diff>
--- a/docs/FCYBL Rankings.xlsx
+++ b/docs/FCYBL Rankings.xlsx
@@ -1220,9 +1220,6 @@
     <t>0.100</t>
   </si>
   <si>
-    <t>FCYBL 2019-2020 Final Regular Season Rankings</t>
-  </si>
-  <si>
     <t>-----</t>
   </si>
   <si>
@@ -1245,6 +1242,9 @@
   </si>
   <si>
     <t>21</t>
+  </si>
+  <si>
+    <t>FCYBL 2019-2020 Regular Season Rankings</t>
   </si>
 </sst>
 </file>
@@ -1697,7 +1697,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>398</v>
+        <v>406</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1718,7 +1718,7 @@
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1729,7 +1729,7 @@
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1745,13 +1745,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2148,7 +2148,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>334</v>
@@ -2206,7 +2206,7 @@
         <v>338</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F28" s="23" t="s">
         <v>337</v>
@@ -2232,7 +2232,7 @@
         <v>338</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F29" s="23" t="s">
         <v>356</v>
@@ -2252,7 +2252,7 @@
         <v>28</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>366</v>
@@ -2313,7 +2313,7 @@
         <v>349</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G32" s="23" t="s">
         <v>341</v>
@@ -2339,7 +2339,7 @@
         <v>349</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G33" s="23" t="s">
         <v>358</v>
@@ -2388,7 +2388,7 @@
         <v>359</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F35" s="23" t="s">
         <v>11</v>
@@ -2469,7 +2469,7 @@
         <v>349</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G38" s="19" t="s">
         <v>339</v>
@@ -2495,7 +2495,7 @@
         <v>349</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G39" s="19" t="s">
         <v>363</v>
@@ -2607,7 +2607,7 @@
         <v>364</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F45" s="23" t="s">
         <v>11</v>
@@ -2659,7 +2659,7 @@
         <v>367</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F47" s="23" t="s">
         <v>392</v>
@@ -2685,10 +2685,10 @@
         <v>367</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G48" s="23" t="s">
         <v>11</v>
@@ -2904,7 +2904,7 @@
         <v>370</v>
       </c>
       <c r="E58" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F58" s="23" t="s">
         <v>337</v>
@@ -2930,7 +2930,7 @@
         <v>370</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F59" s="23" t="s">
         <v>356</v>
@@ -3216,7 +3216,7 @@
         <v>378</v>
       </c>
       <c r="E70" s="16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F70" s="16" t="s">
         <v>11</v>
@@ -5466,7 +5466,7 @@
         <v>374</v>
       </c>
       <c r="E166" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F166" s="23" t="s">
         <v>348</v>
@@ -5492,7 +5492,7 @@
         <v>374</v>
       </c>
       <c r="E167" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F167" s="23" t="s">
         <v>360</v>
@@ -6680,7 +6680,7 @@
         <v>334</v>
       </c>
       <c r="E219" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F219" s="23" t="s">
         <v>341</v>
@@ -6706,7 +6706,7 @@
         <v>334</v>
       </c>
       <c r="E220" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F220" s="23" t="s">
         <v>356</v>
@@ -7482,7 +7482,7 @@
         <v>366</v>
       </c>
       <c r="E253" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F253" s="23" t="s">
         <v>393</v>
@@ -7508,7 +7508,7 @@
         <v>366</v>
       </c>
       <c r="E254" s="23" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F254" s="23" t="s">
         <v>358</v>
@@ -7716,7 +7716,7 @@
         <v>349</v>
       </c>
       <c r="E262" s="16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F262" s="16" t="s">
         <v>337</v>
@@ -7742,7 +7742,7 @@
         <v>349</v>
       </c>
       <c r="E263" s="16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F263" s="16" t="s">
         <v>362</v>

</xml_diff>